<commit_message>
Update XLS array calculation
</commit_message>
<xml_diff>
--- a/trunk/MARMITESutilities/MM_XLSstuff/ArraySize.xlsx
+++ b/trunk/MARMITESutilities/MM_XLSstuff/ArraySize.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python27\WinPython-64bit-2.7.5.3\python-2.7.5.amd64\Lib\site-packages\MARMITES\trunk\MARMITESutilities\MM_XLSstuff\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="23820" windowHeight="12915"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>TS</t>
   </si>
@@ -79,16 +84,28 @@
   </si>
   <si>
     <t>LaMata</t>
+  </si>
+  <si>
+    <t>SOMINCOR_MM</t>
+  </si>
+  <si>
+    <t>SOMINCOR_MM_S</t>
+  </si>
+  <si>
+    <t>SOMINCOR_MM_HEADS32</t>
+  </si>
+  <si>
+    <t>SOMINCOR_MM_HEADS64</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,16 +113,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -113,13 +144,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,6 +179,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -177,7 +230,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,7 +265,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -421,525 +474,682 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>730</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>130</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>60</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>64</v>
-      </c>
-      <c r="H2">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>64</v>
+      </c>
+      <c r="H2" s="1">
         <f t="shared" ref="H2:H8" si="0">B2*C2*D2*E2*F2*G2</f>
         <v>728832000</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <f>H2/1000</f>
         <v>728832</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <f>I2/1000</f>
         <v>728.83199999999999</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="5">
         <f>J2/1000</f>
         <v>0.72883200000000004</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>506</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>130</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>60</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>8</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>32</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <f t="shared" si="0"/>
         <v>2020761600</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <f t="shared" ref="I3:K5" si="1">H3/1000</f>
         <v>2020761.6000000001</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2">
         <f t="shared" si="1"/>
         <v>2020.7616</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="5">
         <f t="shared" si="1"/>
         <v>2.0207616000000002</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>730</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>130</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>60</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
         <v>17</v>
       </c>
-      <c r="G4">
-        <v>64</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="1">
+        <v>64</v>
+      </c>
+      <c r="H4" s="1">
         <f t="shared" si="0"/>
         <v>6195072000</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <f>H4/1000</f>
         <v>6195072</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="2">
         <f>I4/1000</f>
         <v>6195.0720000000001</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="5">
         <f>J4/1000</f>
         <v>6.1950719999999997</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>730</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>130</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>60</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>4</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>6</v>
       </c>
-      <c r="G5">
-        <v>64</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="1">
+        <v>64</v>
+      </c>
+      <c r="H5" s="1">
         <f t="shared" si="0"/>
         <v>8745984000</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <f t="shared" si="1"/>
         <v>8745984</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="2">
         <f t="shared" si="1"/>
         <v>8745.9840000000004</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="5">
         <f t="shared" si="1"/>
         <v>8.745984</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>730</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>130</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>60</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>64</v>
-      </c>
-      <c r="H6">
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>64</v>
+      </c>
+      <c r="H6" s="1">
         <f t="shared" si="0"/>
         <v>364416000</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <f t="shared" ref="I6:I7" si="2">H6/1000</f>
         <v>364416</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="2">
         <f t="shared" ref="J6:J7" si="3">I6/1000</f>
         <v>364.416</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="5">
         <f t="shared" ref="K6:K7" si="4">J6/1000</f>
         <v>0.36441600000000002</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>1565</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>69</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>91</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
         <v>17</v>
       </c>
-      <c r="G7">
-        <v>64</v>
-      </c>
-      <c r="H7">
+      <c r="G7" s="1">
+        <v>64</v>
+      </c>
+      <c r="H7" s="1">
         <f t="shared" si="0"/>
         <v>10691378880</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <f t="shared" si="2"/>
         <v>10691378.880000001</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="2">
         <f t="shared" si="3"/>
         <v>10691.37888</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="5">
         <f t="shared" si="4"/>
         <v>10.69137888</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>1565</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>69</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>91</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>4</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>6</v>
       </c>
-      <c r="G8">
-        <v>64</v>
-      </c>
-      <c r="H8">
+      <c r="G8" s="1">
+        <v>64</v>
+      </c>
+      <c r="H8" s="1">
         <f t="shared" si="0"/>
         <v>15093711360</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <f t="shared" ref="I8" si="5">H8/1000</f>
         <v>15093711.359999999</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="2">
         <f t="shared" ref="J8" si="6">I8/1000</f>
         <v>15093.711359999999</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="5">
         <f t="shared" ref="K8" si="7">J8/1000</f>
         <v>15.093711359999999</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>729</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>131</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>95</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>64</v>
-      </c>
-      <c r="H9">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>64</v>
+      </c>
+      <c r="H9" s="1">
         <f t="shared" ref="H9:H11" si="8">B9*C9*D9*E9*F9*G9</f>
         <v>580633920</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <f t="shared" ref="I9:I11" si="9">H9/1000</f>
         <v>580633.92000000004</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="2">
         <f t="shared" ref="J9:J11" si="10">I9/1000</f>
         <v>580.63391999999999</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="5">
         <f t="shared" ref="K9:K11" si="11">J9/1000</f>
         <v>0.58063392000000003</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>353</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>40</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>20</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>64</v>
-      </c>
-      <c r="H10">
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>64</v>
+      </c>
+      <c r="H10" s="1">
         <f t="shared" si="8"/>
         <v>36147200</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <f t="shared" si="9"/>
         <v>36147.199999999997</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="2">
         <f t="shared" si="10"/>
         <v>36.147199999999998</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="5">
         <f t="shared" si="11"/>
         <v>3.6147199999999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>1887</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>69</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>72</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>7</v>
       </c>
-      <c r="G11">
-        <v>64</v>
-      </c>
-      <c r="H11">
+      <c r="G11" s="1">
+        <v>64</v>
+      </c>
+      <c r="H11" s="1">
         <f t="shared" si="8"/>
         <v>8399655936</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <f t="shared" si="9"/>
         <v>8399655.9360000007</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="2">
         <f t="shared" si="10"/>
         <v>8399.655936000001</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="5">
         <f t="shared" si="11"/>
         <v>8.3996559360000003</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <f>B11/2</f>
         <v>943.5</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>69</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>72</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>7</v>
       </c>
-      <c r="G12">
-        <v>64</v>
-      </c>
-      <c r="H12">
+      <c r="G12" s="1">
+        <v>64</v>
+      </c>
+      <c r="H12" s="1">
         <f t="shared" ref="H12" si="12">B12*C12*D12*E12*F12*G12</f>
         <v>4199827968</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="1">
         <f t="shared" ref="I12" si="13">H12/1000</f>
         <v>4199827.9680000003</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="2">
         <f t="shared" ref="J12" si="14">I12/1000</f>
         <v>4199.8279680000005</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="5">
         <f t="shared" ref="K12" si="15">J12/1000</f>
         <v>4.1998279680000001</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <f>B12/2</f>
         <v>471.75</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>69</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>72</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>7</v>
       </c>
-      <c r="G13">
-        <v>64</v>
-      </c>
-      <c r="H13">
+      <c r="G13" s="1">
+        <v>64</v>
+      </c>
+      <c r="H13" s="1">
         <f t="shared" ref="H13" si="16">B13*C13*D13*E13*F13*G13</f>
         <v>2099913984</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="1">
         <f t="shared" ref="I13" si="17">H13/1000</f>
         <v>2099913.9840000002</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="2">
         <f t="shared" ref="J13" si="18">I13/1000</f>
         <v>2099.9139840000003</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="5">
         <f t="shared" ref="K13" si="19">J13/1000</f>
         <v>2.0999139840000001</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1">
+        <v>813</v>
+      </c>
+      <c r="C14" s="1">
+        <v>270</v>
+      </c>
+      <c r="D14" s="1">
+        <v>260</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>17</v>
+      </c>
+      <c r="G14" s="1">
+        <v>64</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" ref="H14" si="20">B14*C14*D14*E14*F14*G14</f>
+        <v>62094988800</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" ref="I14" si="21">H14/1000</f>
+        <v>62094988.799999997</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" ref="J14" si="22">I14/1000</f>
+        <v>62094.988799999999</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" ref="K14" si="23">J14/1000</f>
+        <v>62.094988799999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1">
+        <v>813</v>
+      </c>
+      <c r="C15" s="1">
+        <v>270</v>
+      </c>
+      <c r="D15" s="1">
+        <v>260</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6</v>
+      </c>
+      <c r="G15" s="1">
+        <v>64</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" ref="H15" si="24">B15*C15*D15*E15*F15*G15</f>
+        <v>65747635200</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" ref="I15" si="25">H15/1000</f>
+        <v>65747635.200000003</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" ref="J15" si="26">I15/1000</f>
+        <v>65747.635200000004</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" ref="K15" si="27">J15/1000</f>
+        <v>65.747635200000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1">
+        <v>813</v>
+      </c>
+      <c r="C16" s="1">
+        <v>270</v>
+      </c>
+      <c r="D16" s="1">
+        <v>260</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>64</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" ref="H16" si="28">B16*C16*D16*E16*F16*G16</f>
+        <v>3652646400</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" ref="I16" si="29">H16/1000</f>
+        <v>3652646.4</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" ref="J16" si="30">I16/1000</f>
+        <v>3652.6464000000001</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" ref="K16" si="31">J16/1000</f>
+        <v>3.6526464000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1">
+        <v>813</v>
+      </c>
+      <c r="C17" s="1">
+        <v>270</v>
+      </c>
+      <c r="D17" s="1">
+        <v>260</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>32</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" ref="H17" si="32">B17*C17*D17*E17*F17*G17</f>
+        <v>1826323200</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" ref="I17" si="33">H17/1000</f>
+        <v>1826323.2</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" ref="J17" si="34">I17/1000</f>
+        <v>1826.3232</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" ref="K17" si="35">J17/1000</f>
+        <v>1.8263232</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
minor change - VERBOSE
VERBOSE in module MMsoil
</commit_message>
<xml_diff>
--- a/trunk/MARMITESutilities/MM_XLSstuff/ArraySize.xlsx
+++ b/trunk/MARMITESutilities/MM_XLSstuff/ArraySize.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python27\WinPython-64bit-2.7.5.3\python-2.7.5.amd64\Lib\site-packages\MARMITES\trunk\MARMITESutilities\MM_XLSstuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python27\201811\Lib\site-packages\MARMITES\trunk\MARMITESutilities\MM_XLSstuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="23820" windowHeight="12915"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="23820" windowHeight="12915" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="SOMINCOR_short" sheetId="2" r:id="rId2"/>
+    <sheet name="SOMINCOR_long" sheetId="4" r:id="rId3"/>
+    <sheet name="SOMINCOR_long_1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
   <si>
     <t>TS</t>
   </si>
@@ -108,6 +109,30 @@
   </si>
   <si>
     <t>SOMINCOR_MM_HEADS64_d</t>
+  </si>
+  <si>
+    <t>H5_file</t>
+  </si>
+  <si>
+    <t>Etg</t>
+  </si>
+  <si>
+    <t>Etg_d</t>
+  </si>
+  <si>
+    <t>PERC</t>
+  </si>
+  <si>
+    <t>PERC_d</t>
+  </si>
+  <si>
+    <t>cbc_MF_d</t>
+  </si>
+  <si>
+    <t>h_MF_d</t>
+  </si>
+  <si>
+    <t>MF</t>
   </si>
 </sst>
 </file>
@@ -148,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -171,17 +196,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,24 +1378,1435 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2496</v>
+      </c>
+      <c r="D2" s="1">
+        <v>270</v>
+      </c>
+      <c r="E2" s="1">
+        <v>260</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:I3" si="0">C2*D2*E2*F2*G2*H2</f>
+        <v>134568345600</v>
+      </c>
+      <c r="J2" s="8">
+        <f t="shared" ref="J2:L2" si="1">I2/1000</f>
+        <v>134568345.59999999</v>
+      </c>
+      <c r="K2" s="8">
+        <f t="shared" si="1"/>
+        <v>134568.3456</v>
+      </c>
+      <c r="L2" s="4">
+        <f t="shared" si="1"/>
+        <v>134.56834559999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2496</v>
+      </c>
+      <c r="D3" s="1">
+        <v>270</v>
+      </c>
+      <c r="E3" s="1">
+        <v>260</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" si="0"/>
+        <v>151389388800</v>
+      </c>
+      <c r="J3" s="8">
+        <f t="shared" ref="J3:L3" si="2">I3/1000</f>
+        <v>151389388.80000001</v>
+      </c>
+      <c r="K3" s="8">
+        <f t="shared" si="2"/>
+        <v>151389.38880000002</v>
+      </c>
+      <c r="L3" s="4">
+        <f t="shared" si="2"/>
+        <v>151.38938880000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1">
+        <v>813</v>
+      </c>
+      <c r="D4" s="1">
+        <v>270</v>
+      </c>
+      <c r="E4" s="1">
+        <v>260</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:I7" si="3">C4*D4*E4*F4*G4*H4</f>
+        <v>1826323200</v>
+      </c>
+      <c r="J4" s="8">
+        <f t="shared" ref="J4:J7" si="4">I4/1000</f>
+        <v>1826323.2</v>
+      </c>
+      <c r="K4" s="8">
+        <f t="shared" ref="K4:K7" si="5">J4/1000</f>
+        <v>1826.3232</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" ref="L4:L7" si="6">K4/1000</f>
+        <v>1.8263232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2496</v>
+      </c>
+      <c r="D5" s="1">
+        <v>270</v>
+      </c>
+      <c r="E5" s="1">
+        <v>260</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="3"/>
+        <v>5607014400</v>
+      </c>
+      <c r="J5" s="8">
+        <f t="shared" si="4"/>
+        <v>5607014.4000000004</v>
+      </c>
+      <c r="K5" s="8">
+        <f t="shared" si="5"/>
+        <v>5607.0144</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" si="6"/>
+        <v>5.6070143999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1">
+        <v>813</v>
+      </c>
+      <c r="D6" s="1">
+        <v>270</v>
+      </c>
+      <c r="E6" s="1">
+        <v>260</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>32</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="3"/>
+        <v>1826323200</v>
+      </c>
+      <c r="J6" s="8">
+        <f t="shared" si="4"/>
+        <v>1826323.2</v>
+      </c>
+      <c r="K6" s="8">
+        <f t="shared" si="5"/>
+        <v>1826.3232</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="6"/>
+        <v>1.8263232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2496</v>
+      </c>
+      <c r="D7" s="1">
+        <v>270</v>
+      </c>
+      <c r="E7" s="1">
+        <v>260</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>32</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="3"/>
+        <v>5607014400</v>
+      </c>
+      <c r="J7" s="8">
+        <f t="shared" si="4"/>
+        <v>5607014.4000000004</v>
+      </c>
+      <c r="K7" s="8">
+        <f t="shared" si="5"/>
+        <v>5607.0144</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="6"/>
+        <v>5.6070143999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J8" s="9">
+        <f>SUM(J2:J7)</f>
+        <v>300824409.5999999</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="7">
+        <f>SUM(L2:L7)</f>
+        <v>300.82440960000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>813</v>
+      </c>
+      <c r="D12" s="1">
+        <v>270</v>
+      </c>
+      <c r="E12" s="1">
+        <v>260</v>
+      </c>
+      <c r="F12" s="1">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>32</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" ref="I12:I13" si="7">C12*D12*E12*F12*G12*H12</f>
+        <v>20089555200</v>
+      </c>
+      <c r="J12" s="1">
+        <f>I12/1000</f>
+        <v>20089555.199999999</v>
+      </c>
+      <c r="K12" s="2">
+        <f>J12/1000</f>
+        <v>20089.555199999999</v>
+      </c>
+      <c r="L12" s="5">
+        <f>K12/1000</f>
+        <v>20.0895552</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>813</v>
+      </c>
+      <c r="D13" s="1">
+        <v>270</v>
+      </c>
+      <c r="E13" s="1">
+        <v>260</v>
+      </c>
+      <c r="F13" s="1">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1">
+        <v>32</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="7"/>
+        <v>160716441600</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" ref="J13:L13" si="8">I13/1000</f>
+        <v>160716441.59999999</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="8"/>
+        <v>160716.44159999999</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="8"/>
+        <v>160.7164416</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2496</v>
+      </c>
+      <c r="D14" s="1">
+        <v>270</v>
+      </c>
+      <c r="E14" s="1">
+        <v>260</v>
+      </c>
+      <c r="F14" s="1">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>32</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" ref="I14:I15" si="9">C14*D14*E14*F14*G14*H14</f>
+        <v>61677158400</v>
+      </c>
+      <c r="J14" s="1">
+        <f>I14/1000</f>
+        <v>61677158.399999999</v>
+      </c>
+      <c r="K14" s="2">
+        <f>J14/1000</f>
+        <v>61677.1584</v>
+      </c>
+      <c r="L14" s="5">
+        <f>K14/1000</f>
+        <v>61.677158400000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2496</v>
+      </c>
+      <c r="D15" s="1">
+        <v>270</v>
+      </c>
+      <c r="E15" s="1">
+        <v>260</v>
+      </c>
+      <c r="F15" s="1">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1">
+        <v>32</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="9"/>
+        <v>493417267200</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" ref="J15" si="10">I15/1000</f>
+        <v>493417267.19999999</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" ref="K15" si="11">J15/1000</f>
+        <v>493417.2672</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" ref="L15" si="12">K15/1000</f>
+        <v>493.41726720000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A12:A15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D2" s="1">
+        <v>270</v>
+      </c>
+      <c r="E2" s="1">
+        <v>260</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:I7" si="0">C2*D2*E2*F2*G2*H2</f>
+        <v>710096025600</v>
+      </c>
+      <c r="J2" s="8">
+        <f t="shared" ref="J2:L7" si="1">I2/1000</f>
+        <v>710096025.60000002</v>
+      </c>
+      <c r="K2" s="8">
+        <f t="shared" si="1"/>
+        <v>710096.02560000005</v>
+      </c>
+      <c r="L2" s="4">
+        <f t="shared" si="1"/>
+        <v>710.09602560000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D3" s="1">
+        <v>270</v>
+      </c>
+      <c r="E3" s="1">
+        <v>260</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" si="0"/>
+        <v>798858028800</v>
+      </c>
+      <c r="J3" s="8">
+        <f t="shared" si="1"/>
+        <v>798858028.79999995</v>
+      </c>
+      <c r="K3" s="8">
+        <f t="shared" si="1"/>
+        <v>798858.02879999997</v>
+      </c>
+      <c r="L3" s="4">
+        <f t="shared" si="1"/>
+        <v>798.85802879999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4338</v>
+      </c>
+      <c r="D4" s="1">
+        <v>270</v>
+      </c>
+      <c r="E4" s="1">
+        <v>260</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>9744883200</v>
+      </c>
+      <c r="J4" s="8">
+        <f t="shared" si="1"/>
+        <v>9744883.1999999993</v>
+      </c>
+      <c r="K4" s="8">
+        <f t="shared" si="1"/>
+        <v>9744.8831999999984</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" si="1"/>
+        <v>9.7448831999999985</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D5" s="1">
+        <v>270</v>
+      </c>
+      <c r="E5" s="1">
+        <v>260</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>29587334400</v>
+      </c>
+      <c r="J5" s="8">
+        <f t="shared" si="1"/>
+        <v>29587334.399999999</v>
+      </c>
+      <c r="K5" s="8">
+        <f t="shared" si="1"/>
+        <v>29587.3344</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" si="1"/>
+        <v>29.5873344</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4338</v>
+      </c>
+      <c r="D6" s="1">
+        <v>270</v>
+      </c>
+      <c r="E6" s="1">
+        <v>260</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>32</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>9744883200</v>
+      </c>
+      <c r="J6" s="8">
+        <f t="shared" si="1"/>
+        <v>9744883.1999999993</v>
+      </c>
+      <c r="K6" s="8">
+        <f t="shared" si="1"/>
+        <v>9744.8831999999984</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="1"/>
+        <v>9.7448831999999985</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D7" s="1">
+        <v>270</v>
+      </c>
+      <c r="E7" s="1">
+        <v>260</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>32</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>29587334400</v>
+      </c>
+      <c r="J7" s="8">
+        <f t="shared" si="1"/>
+        <v>29587334.399999999</v>
+      </c>
+      <c r="K7" s="8">
+        <f t="shared" si="1"/>
+        <v>29587.3344</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="1"/>
+        <v>29.5873344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J8" s="9">
+        <f>SUM(J2:J7)</f>
+        <v>1587618489.6000004</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="7">
+        <f>SUM(L2:L7)</f>
+        <v>1587.6184896</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4338</v>
+      </c>
+      <c r="D12" s="1">
+        <v>270</v>
+      </c>
+      <c r="E12" s="1">
+        <v>260</v>
+      </c>
+      <c r="F12" s="1">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>32</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" ref="I12:I15" si="2">C12*D12*E12*F12*G12*H12</f>
+        <v>107193715200</v>
+      </c>
+      <c r="J12" s="1">
+        <f>I12/1000</f>
+        <v>107193715.2</v>
+      </c>
+      <c r="K12" s="2">
+        <f>J12/1000</f>
+        <v>107193.71520000001</v>
+      </c>
+      <c r="L12" s="5">
+        <f>K12/1000</f>
+        <v>107.1937152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4338</v>
+      </c>
+      <c r="D13" s="1">
+        <v>270</v>
+      </c>
+      <c r="E13" s="1">
+        <v>260</v>
+      </c>
+      <c r="F13" s="1">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1">
+        <v>32</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="2"/>
+        <v>857549721600</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" ref="J13:L13" si="3">I13/1000</f>
+        <v>857549721.60000002</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>857549.72160000005</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="3"/>
+        <v>857.5497216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D14" s="1">
+        <v>270</v>
+      </c>
+      <c r="E14" s="1">
+        <v>260</v>
+      </c>
+      <c r="F14" s="1">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>32</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="2"/>
+        <v>325460678400</v>
+      </c>
+      <c r="J14" s="1">
+        <f>I14/1000</f>
+        <v>325460678.39999998</v>
+      </c>
+      <c r="K14" s="2">
+        <f>J14/1000</f>
+        <v>325460.67839999998</v>
+      </c>
+      <c r="L14" s="5">
+        <f>K14/1000</f>
+        <v>325.46067839999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D15" s="1">
+        <v>270</v>
+      </c>
+      <c r="E15" s="1">
+        <v>260</v>
+      </c>
+      <c r="F15" s="1">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1">
+        <v>32</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="2"/>
+        <v>2603685427200</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" ref="J15:L15" si="4">I15/1000</f>
+        <v>2603685427.1999998</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="4"/>
+        <v>2603685.4271999998</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" si="4"/>
+        <v>2603.6854271999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A12:A15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D2" s="1">
+        <v>270</v>
+      </c>
+      <c r="E2" s="1">
+        <v>260</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:I7" si="0">C2*D2*E2*F2*G2*H2</f>
+        <v>710096025600</v>
+      </c>
+      <c r="J2" s="8">
+        <f t="shared" ref="J2:L7" si="1">I2/1000</f>
+        <v>710096025.60000002</v>
+      </c>
+      <c r="K2" s="8">
+        <f t="shared" si="1"/>
+        <v>710096.02560000005</v>
+      </c>
+      <c r="L2" s="4">
+        <f t="shared" si="1"/>
+        <v>710.09602560000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D3" s="1">
+        <v>270</v>
+      </c>
+      <c r="E3" s="1">
+        <v>260</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" si="0"/>
+        <v>798858028800</v>
+      </c>
+      <c r="J3" s="8">
+        <f t="shared" si="1"/>
+        <v>798858028.79999995</v>
+      </c>
+      <c r="K3" s="8">
+        <f t="shared" si="1"/>
+        <v>798858.02879999997</v>
+      </c>
+      <c r="L3" s="4">
+        <f t="shared" si="1"/>
+        <v>798.85802879999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3689</v>
+      </c>
+      <c r="D4" s="1">
+        <v>270</v>
+      </c>
+      <c r="E4" s="1">
+        <v>260</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>8286969600</v>
+      </c>
+      <c r="J4" s="8">
+        <f t="shared" si="1"/>
+        <v>8286969.5999999996</v>
+      </c>
+      <c r="K4" s="8">
+        <f t="shared" si="1"/>
+        <v>8286.9696000000004</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" si="1"/>
+        <v>8.2869696000000008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D5" s="1">
+        <v>270</v>
+      </c>
+      <c r="E5" s="1">
+        <v>260</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>29587334400</v>
+      </c>
+      <c r="J5" s="8">
+        <f t="shared" si="1"/>
+        <v>29587334.399999999</v>
+      </c>
+      <c r="K5" s="8">
+        <f t="shared" si="1"/>
+        <v>29587.3344</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" si="1"/>
+        <v>29.5873344</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3689</v>
+      </c>
+      <c r="D6" s="1">
+        <v>270</v>
+      </c>
+      <c r="E6" s="1">
+        <v>260</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>32</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>8286969600</v>
+      </c>
+      <c r="J6" s="8">
+        <f t="shared" si="1"/>
+        <v>8286969.5999999996</v>
+      </c>
+      <c r="K6" s="8">
+        <f t="shared" si="1"/>
+        <v>8286.9696000000004</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="1"/>
+        <v>8.2869696000000008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D7" s="1">
+        <v>270</v>
+      </c>
+      <c r="E7" s="1">
+        <v>260</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>32</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>29587334400</v>
+      </c>
+      <c r="J7" s="8">
+        <f t="shared" si="1"/>
+        <v>29587334.399999999</v>
+      </c>
+      <c r="K7" s="8">
+        <f t="shared" si="1"/>
+        <v>29587.3344</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="1"/>
+        <v>29.5873344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J8" s="9">
+        <f>SUM(J2:J7)</f>
+        <v>1584702662.4000001</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="7">
+        <f>SUM(L2:L7)</f>
+        <v>1584.7026624</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3689</v>
+      </c>
+      <c r="D12" s="1">
+        <v>270</v>
+      </c>
+      <c r="E12" s="1">
+        <v>260</v>
+      </c>
+      <c r="F12" s="1">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>32</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" ref="I12:I15" si="2">C12*D12*E12*F12*G12*H12</f>
+        <v>91156665600</v>
+      </c>
+      <c r="J12" s="1">
+        <f>I12/1000</f>
+        <v>91156665.599999994</v>
+      </c>
+      <c r="K12" s="2">
+        <f>J12/1000</f>
+        <v>91156.665599999993</v>
+      </c>
+      <c r="L12" s="5">
+        <f>K12/1000</f>
+        <v>91.156665599999997</v>
+      </c>
+      <c r="M12">
+        <f>L12/3</f>
+        <v>30.385555199999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3689</v>
+      </c>
+      <c r="D13" s="1">
+        <v>270</v>
+      </c>
+      <c r="E13" s="1">
+        <v>260</v>
+      </c>
+      <c r="F13" s="1">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1">
+        <v>32</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="2"/>
+        <v>729253324800</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" ref="J13:L13" si="3">I13/1000</f>
+        <v>729253324.79999995</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>729253.32479999994</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="3"/>
+        <v>729.25332479999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D14" s="1">
+        <v>270</v>
+      </c>
+      <c r="E14" s="1">
+        <v>260</v>
+      </c>
+      <c r="F14" s="1">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>32</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="2"/>
+        <v>325460678400</v>
+      </c>
+      <c r="J14" s="1">
+        <f>I14/1000</f>
+        <v>325460678.39999998</v>
+      </c>
+      <c r="K14" s="2">
+        <f>J14/1000</f>
+        <v>325460.67839999998</v>
+      </c>
+      <c r="L14" s="5">
+        <f>K14/1000</f>
+        <v>325.46067839999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1">
+        <v>13171</v>
+      </c>
+      <c r="D15" s="1">
+        <v>270</v>
+      </c>
+      <c r="E15" s="1">
+        <v>260</v>
+      </c>
+      <c r="F15" s="1">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1">
+        <v>32</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="2"/>
+        <v>2603685427200</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" ref="J15:L15" si="4">I15/1000</f>
+        <v>2603685427.1999998</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="4"/>
+        <v>2603685.4271999998</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" si="4"/>
+        <v>2603.6854271999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A12:A15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MAIN UPGRADE 2.7 to 3.8
Upgrade from Python 2.7 to 3.8
</commit_message>
<xml_diff>
--- a/trunk/MARMITESutilities/MM_XLSstuff/ArraySize.xlsx
+++ b/trunk/MARMITESutilities/MM_XLSstuff/ArraySize.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="23820" windowHeight="12915" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="23820" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
   <si>
     <t>TS</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>MF</t>
+  </si>
+  <si>
+    <t>SOMINCOR_MM_HEADS32_d_long</t>
+  </si>
+  <si>
+    <t>SOMINCOR_MM_HEADS32_long</t>
+  </si>
+  <si>
+    <t>SOMINCOR_h_MF_d_long</t>
+  </si>
+  <si>
+    <t>SOMINCOR_h_MF_long</t>
   </si>
 </sst>
 </file>
@@ -541,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,6 +1382,162 @@
         <v>22.428057599999999</v>
       </c>
     </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3696</v>
+      </c>
+      <c r="C22" s="1">
+        <v>270</v>
+      </c>
+      <c r="D22" s="1">
+        <v>260</v>
+      </c>
+      <c r="E22" s="1">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>32</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" ref="H22" si="44">B22*C22*D22*E22*F22*G22</f>
+        <v>33210777600</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" ref="I22" si="45">H22/1000</f>
+        <v>33210777.600000001</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" ref="J22" si="46">I22/1000</f>
+        <v>33210.777600000001</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" ref="K22" si="47">J22/1000</f>
+        <v>33.2107776</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="1">
+        <v>13171</v>
+      </c>
+      <c r="C23" s="1">
+        <v>270</v>
+      </c>
+      <c r="D23" s="1">
+        <v>260</v>
+      </c>
+      <c r="E23" s="1">
+        <v>4</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>32</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" ref="H23:H24" si="48">B23*C23*D23*E23*F23*G23</f>
+        <v>118349337600</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" ref="I23" si="49">H23/1000</f>
+        <v>118349337.59999999</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" ref="J23" si="50">I23/1000</f>
+        <v>118349.3376</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" ref="K23" si="51">J23/1000</f>
+        <v>118.3493376</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3696</v>
+      </c>
+      <c r="C24" s="1">
+        <v>270</v>
+      </c>
+      <c r="D24" s="1">
+        <v>260</v>
+      </c>
+      <c r="E24" s="1">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>32</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="48"/>
+        <v>83026944000</v>
+      </c>
+      <c r="I24" s="1">
+        <f>H24/1000</f>
+        <v>83026944</v>
+      </c>
+      <c r="J24" s="2">
+        <f>I24/1000</f>
+        <v>83026.944000000003</v>
+      </c>
+      <c r="K24" s="5">
+        <f>J24/1000</f>
+        <v>83.026944</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1">
+        <v>13171</v>
+      </c>
+      <c r="C25" s="1">
+        <v>270</v>
+      </c>
+      <c r="D25" s="1">
+        <v>260</v>
+      </c>
+      <c r="E25" s="1">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>32</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25" si="52">B25*C25*D25*E25*F25*G25</f>
+        <v>295873344000</v>
+      </c>
+      <c r="I25" s="1">
+        <f>H25/1000</f>
+        <v>295873344</v>
+      </c>
+      <c r="J25" s="2">
+        <f>I25/1000</f>
+        <v>295873.34399999998</v>
+      </c>
+      <c r="K25" s="5">
+        <f>J25/1000</f>
+        <v>295.87334399999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1380,9 +1548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1858,7 +2024,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,9 +2500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>